<commit_message>
Changed reference designators to nominal, added missing OOI Barcodes
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GP03FLMB_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_GP03FLMB_00002.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\IRAD\IRAD 2015\Programs\OOI Phase 2\Post Delivery 7 support\Asset Management Data\ingestion-csvs_20151204\ingestion-csvs\GP_mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="1944" windowWidth="24960" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="2310" yWindow="1950" windowWidth="24960" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="118">
   <si>
     <t>Ref Des</t>
   </si>
@@ -232,42 +232,6 @@
     <t>GP03FLMB-RIM01-02-ADCPSL007</t>
   </si>
   <si>
-    <t>GP03FLMB-RIM01-02-CTDMOG046</t>
-  </si>
-  <si>
-    <t>GP03FLMB-RIM01-02-CTDMOG053</t>
-  </si>
-  <si>
-    <t>GP03FLMB-RIM01-02-CTDMOG041</t>
-  </si>
-  <si>
-    <t>GP03FLMB-RIM01-02-CTDMOG050</t>
-  </si>
-  <si>
-    <t>GP03FLMB-RIM01-02-CTDMOG038</t>
-  </si>
-  <si>
-    <t>GP03FLMB-RIM01-02-CTDMOG040</t>
-  </si>
-  <si>
-    <t>GP03FLMB-RIM01-02-CTDMOG039</t>
-  </si>
-  <si>
-    <t>GP03FLMB-RIM01-02-CTDMOG023</t>
-  </si>
-  <si>
-    <t>GP03FLMB-RIM01-02-CTDMOG054</t>
-  </si>
-  <si>
-    <t>GP03FLMB-RIM01-02-CTDMOH028</t>
-  </si>
-  <si>
-    <t>GP03FLMB-RIM01-02-CTDMOH080</t>
-  </si>
-  <si>
-    <t>GP03FLMB-RIM01-02-CTDMOH003</t>
-  </si>
-  <si>
     <t>GP03FLMA-00001</t>
   </si>
   <si>
@@ -278,6 +242,102 @@
   </si>
   <si>
     <t>MV-1404</t>
+  </si>
+  <si>
+    <t>Units in mm</t>
+  </si>
+  <si>
+    <t>Mooring OOIBARCODE</t>
+  </si>
+  <si>
+    <t>Sensor OOIBARCODE</t>
+  </si>
+  <si>
+    <t>N00254</t>
+  </si>
+  <si>
+    <t>A00467</t>
+  </si>
+  <si>
+    <t>A01501</t>
+  </si>
+  <si>
+    <t>A00413</t>
+  </si>
+  <si>
+    <t>A00570</t>
+  </si>
+  <si>
+    <t>37-11646</t>
+  </si>
+  <si>
+    <t>A01398</t>
+  </si>
+  <si>
+    <t>37-11654</t>
+  </si>
+  <si>
+    <t>A01406</t>
+  </si>
+  <si>
+    <t>37-11653</t>
+  </si>
+  <si>
+    <t>A01405</t>
+  </si>
+  <si>
+    <t>A01393</t>
+  </si>
+  <si>
+    <t>37-11641</t>
+  </si>
+  <si>
+    <t>A01402</t>
+  </si>
+  <si>
+    <t>37-11650</t>
+  </si>
+  <si>
+    <t>37-11638</t>
+  </si>
+  <si>
+    <t>A01390</t>
+  </si>
+  <si>
+    <t>A01392</t>
+  </si>
+  <si>
+    <t>37-11640</t>
+  </si>
+  <si>
+    <t>37-11639</t>
+  </si>
+  <si>
+    <t>A01391</t>
+  </si>
+  <si>
+    <t>37-10223</t>
+  </si>
+  <si>
+    <t>A00112</t>
+  </si>
+  <si>
+    <t>37-10228</t>
+  </si>
+  <si>
+    <t>A00135</t>
+  </si>
+  <si>
+    <t>37-11680</t>
+  </si>
+  <si>
+    <t>A01407</t>
+  </si>
+  <si>
+    <t>37-11703</t>
+  </si>
+  <si>
+    <t>A01411</t>
   </si>
   <si>
     <r>
@@ -300,7 +360,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>M01-01-SIOENG000</t>
+      <t>M01-00-SIOENG000</t>
     </r>
   </si>
   <si>
@@ -324,104 +384,50 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>S01-01-SIOENG000</t>
+      <t>S01-00-SIOENG000</t>
     </r>
   </si>
   <si>
-    <t>Units in mm</t>
-  </si>
-  <si>
-    <t>Mooring OOIBARCODE</t>
-  </si>
-  <si>
-    <t>Sensor OOIBARCODE</t>
-  </si>
-  <si>
-    <t>N00254</t>
-  </si>
-  <si>
-    <t>A00467</t>
-  </si>
-  <si>
-    <t>A01501</t>
-  </si>
-  <si>
-    <t>A00413</t>
-  </si>
-  <si>
-    <t>A00570</t>
-  </si>
-  <si>
-    <t>37-11646</t>
-  </si>
-  <si>
-    <t>A01398</t>
-  </si>
-  <si>
-    <t>37-11654</t>
-  </si>
-  <si>
-    <t>A01406</t>
-  </si>
-  <si>
-    <t>37-11653</t>
-  </si>
-  <si>
-    <t>A01405</t>
-  </si>
-  <si>
-    <t>A01393</t>
-  </si>
-  <si>
-    <t>37-11641</t>
-  </si>
-  <si>
-    <t>A01402</t>
-  </si>
-  <si>
-    <t>37-11650</t>
-  </si>
-  <si>
-    <t>37-11638</t>
-  </si>
-  <si>
-    <t>A01390</t>
-  </si>
-  <si>
-    <t>A01392</t>
-  </si>
-  <si>
-    <t>37-11640</t>
-  </si>
-  <si>
-    <t>37-11639</t>
-  </si>
-  <si>
-    <t>A01391</t>
-  </si>
-  <si>
-    <t>37-10223</t>
-  </si>
-  <si>
-    <t>A00112</t>
-  </si>
-  <si>
-    <t>37-10228</t>
-  </si>
-  <si>
-    <t>A00135</t>
-  </si>
-  <si>
-    <t>37-11680</t>
-  </si>
-  <si>
-    <t>A01407</t>
-  </si>
-  <si>
-    <t>37-11703</t>
-  </si>
-  <si>
-    <t>A01411</t>
+    <t>GP03FLMB-RIM01-02-CTDMOG060</t>
+  </si>
+  <si>
+    <t>GP03FLMB-RIM01-02-CTDMOG068</t>
+  </si>
+  <si>
+    <t>GP03FLMB-RIM01-02-CTDMOG061</t>
+  </si>
+  <si>
+    <t>GP03FLMB-RIM01-02-CTDMOG062</t>
+  </si>
+  <si>
+    <t>GP03FLMB-RIM01-02-CTDMOG063</t>
+  </si>
+  <si>
+    <t>GP03FLMB-RIM01-02-CTDMOG064</t>
+  </si>
+  <si>
+    <t>GP03FLMB-RIM01-02-CTDMOG065</t>
+  </si>
+  <si>
+    <t>GP03FLMB-RIM01-02-CTDMOG067</t>
+  </si>
+  <si>
+    <t>GP03FLMB-RIM01-02-CTDMOG066</t>
+  </si>
+  <si>
+    <t>GP03FLMB-RIM01-02-CTDMOH069</t>
+  </si>
+  <si>
+    <t>GP03FLMB-RIM01-02-CTDMOH070</t>
+  </si>
+  <si>
+    <t>GP03FLMB-RIM01-02-CTDMOH071</t>
+  </si>
+  <si>
+    <t>OL000102</t>
+  </si>
+  <si>
+    <t>OL000103</t>
   </si>
 </sst>
 </file>
@@ -911,7 +917,7 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1009,17 +1015,11 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="60" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1057,6 +1057,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="134">
@@ -1518,60 +1521,60 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.44140625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" style="6" customWidth="1"/>
-    <col min="15" max="16384" width="8.77734375" style="6"/>
+    <col min="8" max="8" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="6" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="8.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="7" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="48" t="s">
+    <row r="1" spans="1:16" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="K1" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="46" t="s">
         <v>37</v>
       </c>
       <c r="M1" s="28" t="s">
@@ -1587,11 +1590,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -1606,7 +1609,7 @@
       <c r="F2" s="25">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="G2" s="45">
+      <c r="G2" s="43">
         <v>42162</v>
       </c>
       <c r="H2" s="5" t="s">
@@ -1618,8 +1621,8 @@
       <c r="J2" s="5">
         <v>4145</v>
       </c>
-      <c r="K2" s="44" t="s">
-        <v>81</v>
+      <c r="K2" s="42" t="s">
+        <v>69</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="26">
@@ -1637,12 +1640,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E3" s="22"/>
       <c r="F3" s="23"/>
       <c r="G3" s="22"/>
     </row>
-    <row r="4" spans="1:16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="24"/>
     </row>
   </sheetData>
@@ -1658,37 +1661,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O84"/>
+  <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E76" sqref="E76:E79"/>
+      <selection pane="bottomRight" activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="8" customWidth="1"/>
-    <col min="10" max="13" width="10.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="8" customWidth="1"/>
+    <col min="10" max="13" width="10.7109375" style="2" customWidth="1"/>
     <col min="14" max="14" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.77734375" style="2"/>
+    <col min="15" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
-        <v>85</v>
+      <c r="B1" s="47" t="s">
+        <v>71</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>1</v>
@@ -1696,8 +1699,8 @@
       <c r="D1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="49" t="s">
-        <v>86</v>
+      <c r="E1" s="47" t="s">
+        <v>72</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>2</v>
@@ -1718,7 +1721,7 @@
       <c r="N1" s="19"/>
       <c r="O1" s="19"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
@@ -1735,12 +1738,12 @@
       <c r="N2" s="20"/>
       <c r="O2" s="20"/>
     </row>
-    <row r="3" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>48</v>
@@ -1749,7 +1752,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F3" s="5">
         <v>1124</v>
@@ -1768,12 +1771,12 @@
       </c>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C4" s="29" t="s">
         <v>48</v>
@@ -1782,7 +1785,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F4" s="29">
         <v>1124</v>
@@ -1798,12 +1801,12 @@
       </c>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C5" s="29" t="s">
         <v>48</v>
@@ -1812,7 +1815,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F5" s="29">
         <v>1124</v>
@@ -1825,12 +1828,12 @@
       </c>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>48</v>
@@ -1839,7 +1842,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F6" s="29">
         <v>1124</v>
@@ -1852,12 +1855,12 @@
       </c>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>48</v>
@@ -1866,7 +1869,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F7" s="29">
         <v>1124</v>
@@ -1879,12 +1882,12 @@
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C8" s="29" t="s">
         <v>48</v>
@@ -1893,7 +1896,7 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F8" s="29">
         <v>1124</v>
@@ -1906,12 +1909,12 @@
       </c>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C9" s="29" t="s">
         <v>48</v>
@@ -1920,7 +1923,7 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F9" s="29">
         <v>1124</v>
@@ -1936,12 +1939,12 @@
       </c>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>48</v>
@@ -1950,7 +1953,7 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F10" s="29">
         <v>1124</v>
@@ -1966,12 +1969,12 @@
       </c>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C11" s="29" t="s">
         <v>48</v>
@@ -1980,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F11" s="29">
         <v>1124</v>
@@ -1996,12 +1999,12 @@
       </c>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C12" s="29" t="s">
         <v>48</v>
@@ -2010,7 +2013,7 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F12" s="29">
         <v>1124</v>
@@ -2026,12 +2029,12 @@
       </c>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>48</v>
@@ -2040,7 +2043,7 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>60</v>
@@ -2059,12 +2062,12 @@
       </c>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C14" s="29" t="s">
         <v>48</v>
@@ -2073,7 +2076,7 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F14" s="29" t="s">
         <v>60</v>
@@ -2086,12 +2089,12 @@
       </c>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C15" s="29" t="s">
         <v>48</v>
@@ -2100,7 +2103,7 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F15" s="29" t="s">
         <v>60</v>
@@ -2113,12 +2116,12 @@
       </c>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C16" s="29" t="s">
         <v>48</v>
@@ -2127,7 +2130,7 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F16" s="29" t="s">
         <v>60</v>
@@ -2140,12 +2143,12 @@
       </c>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C17" s="29" t="s">
         <v>48</v>
@@ -2154,7 +2157,7 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F17" s="29" t="s">
         <v>60</v>
@@ -2167,12 +2170,12 @@
       </c>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C18" s="29" t="s">
         <v>48</v>
@@ -2181,7 +2184,7 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F18" s="29" t="s">
         <v>60</v>
@@ -2194,12 +2197,12 @@
       </c>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C19" s="29" t="s">
         <v>48</v>
@@ -2208,7 +2211,7 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F19" s="29" t="s">
         <v>60</v>
@@ -2224,12 +2227,12 @@
       </c>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>48</v>
@@ -2238,7 +2241,7 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F20" s="5">
         <v>224</v>
@@ -2257,12 +2260,12 @@
       </c>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C21" s="29" t="s">
         <v>48</v>
@@ -2271,7 +2274,7 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F21" s="29">
         <v>224</v>
@@ -2287,12 +2290,12 @@
       </c>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C22" s="29" t="s">
         <v>48</v>
@@ -2301,7 +2304,7 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F22" s="29">
         <v>224</v>
@@ -2314,12 +2317,12 @@
       </c>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>48</v>
@@ -2328,7 +2331,7 @@
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F23" s="5">
         <v>20504</v>
@@ -2347,12 +2350,12 @@
       </c>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C24" s="29" t="s">
         <v>48</v>
@@ -2361,7 +2364,7 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F24" s="29">
         <v>20504</v>
@@ -2374,12 +2377,12 @@
       </c>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
         <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C25" s="29" t="s">
         <v>48</v>
@@ -2388,12 +2391,12 @@
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F25" s="29">
         <v>20504</v>
       </c>
-      <c r="G25" s="38" t="s">
+      <c r="G25" s="36" t="s">
         <v>8</v>
       </c>
       <c r="H25" s="4">
@@ -2401,12 +2404,12 @@
       </c>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
         <v>65</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C26" s="29" t="s">
         <v>48</v>
@@ -2415,12 +2418,12 @@
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F26" s="29">
         <v>20504</v>
       </c>
-      <c r="G26" s="38" t="s">
+      <c r="G26" s="36" t="s">
         <v>9</v>
       </c>
       <c r="H26" s="4">
@@ -2428,12 +2431,12 @@
       </c>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
         <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C27" s="29" t="s">
         <v>48</v>
@@ -2442,7 +2445,7 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F27" s="29">
         <v>20504</v>
@@ -2450,20 +2453,20 @@
       <c r="G27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H27" s="46">
+      <c r="H27" s="44">
         <v>500000</v>
       </c>
-      <c r="I27" s="47" t="s">
-        <v>84</v>
+      <c r="I27" s="45" t="s">
+        <v>70</v>
       </c>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
         <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C28" s="29" t="s">
         <v>48</v>
@@ -2472,7 +2475,7 @@
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F28" s="29">
         <v>20504</v>
@@ -2485,12 +2488,12 @@
       </c>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
         <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C29" s="29" t="s">
         <v>48</v>
@@ -2499,7 +2502,7 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F29" s="29">
         <v>20504</v>
@@ -2512,12 +2515,12 @@
       </c>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
         <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C30" s="29" t="s">
         <v>48</v>
@@ -2526,7 +2529,7 @@
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F30" s="29">
         <v>20504</v>
@@ -2539,12 +2542,12 @@
       </c>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
         <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C31" s="29" t="s">
         <v>48</v>
@@ -2553,7 +2556,7 @@
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F31" s="29">
         <v>20504</v>
@@ -2566,12 +2569,12 @@
       </c>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="31" t="s">
-        <v>66</v>
+    <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>48</v>
@@ -2580,10 +2583,10 @@
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F32" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>5</v>
@@ -2598,12 +2601,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="30" t="s">
-        <v>66</v>
+    <row r="33" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>104</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C33" s="29" t="s">
         <v>48</v>
@@ -2612,10 +2615,10 @@
         <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F33" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>6</v>
@@ -2624,12 +2627,12 @@
         <v>50.331333333333333</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="30" t="s">
-        <v>66</v>
+    <row r="34" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C34" s="29" t="s">
         <v>48</v>
@@ -2638,10 +2641,10 @@
         <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F34" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>7</v>
@@ -2650,12 +2653,12 @@
         <v>-144.39750000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="30" t="s">
-        <v>66</v>
+    <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C35" s="29" t="s">
         <v>48</v>
@@ -2664,10 +2667,10 @@
         <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F35" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>57</v>
@@ -2676,472 +2679,395 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36" s="29"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="8">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" t="s">
+        <v>80</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="4">
+        <v>1450</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="8">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" t="s">
+        <v>80</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H38" s="4">
+        <v>50.331333333333333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="8">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>81</v>
+      </c>
+      <c r="F39" t="s">
+        <v>80</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="4">
+        <v>-144.39750000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="8">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" t="s">
+        <v>80</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H40" s="4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41" s="29"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="8">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>83</v>
+      </c>
+      <c r="F42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H42" s="4">
+        <v>1450</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="8">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>83</v>
+      </c>
+      <c r="F43" t="s">
+        <v>82</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" s="4">
+        <v>50.331333333333333</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="8">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>83</v>
+      </c>
+      <c r="F44" t="s">
+        <v>82</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" s="4">
+        <v>-144.39750000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="8">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>83</v>
+      </c>
+      <c r="F45" t="s">
+        <v>82</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H45" s="4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46"/>
+      <c r="B46"/>
+      <c r="C46" s="29"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="8">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>84</v>
+      </c>
+      <c r="F47" t="s">
+        <v>85</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H47" s="4">
+        <v>1450</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47" s="5">
+        <v>90</v>
+      </c>
+      <c r="L47" s="5"/>
+    </row>
+    <row r="48" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="8">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>84</v>
+      </c>
+      <c r="F48" t="s">
+        <v>85</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H48" s="4">
+        <v>50.331333333333333</v>
+      </c>
+      <c r="L48" s="5"/>
+    </row>
+    <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="8">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>84</v>
+      </c>
+      <c r="F49" t="s">
+        <v>85</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" s="4">
+        <v>-144.39750000000001</v>
+      </c>
+      <c r="L49" s="5"/>
+    </row>
+    <row r="50" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" s="8">
+        <v>2</v>
+      </c>
+      <c r="E50" t="s">
+        <v>84</v>
+      </c>
+      <c r="F50" t="s">
+        <v>85</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H50" s="4">
+        <v>41</v>
+      </c>
+      <c r="L50" s="5"/>
+    </row>
+    <row r="51" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51"/>
+      <c r="B51"/>
+      <c r="C51" s="29"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="L51" s="5"/>
+    </row>
+    <row r="52" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52" s="8">
+        <v>2</v>
+      </c>
+      <c r="E52" t="s">
+        <v>86</v>
+      </c>
+      <c r="F52" t="s">
         <v>87</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="8">
-        <v>2</v>
-      </c>
-      <c r="E36" t="s">
-        <v>95</v>
-      </c>
-      <c r="F36" t="s">
-        <v>94</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H36" s="4">
-        <v>1450</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J36" s="5">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="B37" t="s">
-        <v>87</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="8">
-        <v>2</v>
-      </c>
-      <c r="E37" t="s">
-        <v>95</v>
-      </c>
-      <c r="F37" t="s">
-        <v>94</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H37" s="4">
-        <v>50.331333333333333</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" s="8">
-        <v>2</v>
-      </c>
-      <c r="E38" t="s">
-        <v>95</v>
-      </c>
-      <c r="F38" t="s">
-        <v>94</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H38" s="4">
-        <v>-144.39750000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" t="s">
-        <v>87</v>
-      </c>
-      <c r="C39" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D39" s="8">
-        <v>2</v>
-      </c>
-      <c r="E39" t="s">
-        <v>95</v>
-      </c>
-      <c r="F39" t="s">
-        <v>94</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H39" s="4">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="8">
-        <v>2</v>
-      </c>
-      <c r="E40" t="s">
-        <v>97</v>
-      </c>
-      <c r="F40" t="s">
-        <v>96</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H40" s="4">
-        <v>1450</v>
-      </c>
-      <c r="I40" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J40" s="5">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="8">
-        <v>2</v>
-      </c>
-      <c r="E41" t="s">
-        <v>97</v>
-      </c>
-      <c r="F41" t="s">
-        <v>96</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H41" s="4">
-        <v>50.331333333333333</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="8">
-        <v>2</v>
-      </c>
-      <c r="E42" t="s">
-        <v>97</v>
-      </c>
-      <c r="F42" t="s">
-        <v>96</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" s="4">
-        <v>-144.39750000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" t="s">
-        <v>87</v>
-      </c>
-      <c r="C43" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D43" s="8">
-        <v>2</v>
-      </c>
-      <c r="E43" t="s">
-        <v>97</v>
-      </c>
-      <c r="F43" t="s">
-        <v>96</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H43" s="4">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B44" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44" s="8">
-        <v>2</v>
-      </c>
-      <c r="E44" t="s">
-        <v>98</v>
-      </c>
-      <c r="F44" t="s">
-        <v>99</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H44" s="4">
-        <v>1450</v>
-      </c>
-      <c r="I44" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J44" s="5">
-        <v>90</v>
-      </c>
-      <c r="L44" s="5"/>
-    </row>
-    <row r="45" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B45" t="s">
-        <v>87</v>
-      </c>
-      <c r="C45" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D45" s="8">
-        <v>2</v>
-      </c>
-      <c r="E45" t="s">
-        <v>98</v>
-      </c>
-      <c r="F45" t="s">
-        <v>99</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H45" s="4">
-        <v>50.331333333333333</v>
-      </c>
-      <c r="L45" s="5"/>
-    </row>
-    <row r="46" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B46" t="s">
-        <v>87</v>
-      </c>
-      <c r="C46" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" s="8">
-        <v>2</v>
-      </c>
-      <c r="E46" t="s">
-        <v>98</v>
-      </c>
-      <c r="F46" t="s">
-        <v>99</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H46" s="4">
-        <v>-144.39750000000001</v>
-      </c>
-      <c r="L46" s="5"/>
-    </row>
-    <row r="47" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B47" t="s">
-        <v>87</v>
-      </c>
-      <c r="C47" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D47" s="8">
-        <v>2</v>
-      </c>
-      <c r="E47" t="s">
-        <v>98</v>
-      </c>
-      <c r="F47" t="s">
-        <v>99</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H47" s="4">
-        <v>41</v>
-      </c>
-      <c r="L47" s="5"/>
-    </row>
-    <row r="48" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="B48" t="s">
-        <v>87</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D48" s="8">
-        <v>2</v>
-      </c>
-      <c r="E48" t="s">
-        <v>100</v>
-      </c>
-      <c r="F48" t="s">
-        <v>101</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H48" s="4">
-        <v>1450</v>
-      </c>
-      <c r="I48" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J48" s="5">
-        <v>130</v>
-      </c>
-      <c r="L48" s="5"/>
-    </row>
-    <row r="49" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="B49" t="s">
-        <v>87</v>
-      </c>
-      <c r="C49" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D49" s="8">
-        <v>2</v>
-      </c>
-      <c r="E49" t="s">
-        <v>100</v>
-      </c>
-      <c r="F49" t="s">
-        <v>101</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H49" s="4">
-        <v>50.331333333333333</v>
-      </c>
-      <c r="L49" s="5"/>
-    </row>
-    <row r="50" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="B50" t="s">
-        <v>87</v>
-      </c>
-      <c r="C50" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D50" s="8">
-        <v>2</v>
-      </c>
-      <c r="E50" t="s">
-        <v>100</v>
-      </c>
-      <c r="F50" t="s">
-        <v>101</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" s="4">
-        <v>-144.39750000000001</v>
-      </c>
-      <c r="L50" s="5"/>
-    </row>
-    <row r="51" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="B51" t="s">
-        <v>87</v>
-      </c>
-      <c r="C51" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D51" s="8">
-        <v>2</v>
-      </c>
-      <c r="E51" t="s">
-        <v>100</v>
-      </c>
-      <c r="F51" t="s">
-        <v>101</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H51" s="4">
-        <v>50</v>
-      </c>
-      <c r="L51" s="5"/>
-    </row>
-    <row r="52" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="B52" t="s">
-        <v>87</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D52" s="8">
-        <v>2</v>
-      </c>
-      <c r="E52" t="s">
-        <v>103</v>
-      </c>
-      <c r="F52" t="s">
-        <v>102</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>5</v>
@@ -3153,28 +3079,28 @@
         <v>14</v>
       </c>
       <c r="J52" s="5">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="30" t="s">
-        <v>71</v>
+    <row r="53" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>108</v>
       </c>
       <c r="B53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D53" s="8">
+        <v>2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>86</v>
+      </c>
+      <c r="F53" t="s">
         <v>87</v>
-      </c>
-      <c r="C53" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D53" s="8">
-        <v>2</v>
-      </c>
-      <c r="E53" t="s">
-        <v>103</v>
-      </c>
-      <c r="F53" t="s">
-        <v>102</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>6</v>
@@ -3184,24 +3110,24 @@
       </c>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="30" t="s">
-        <v>71</v>
+    <row r="54" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>108</v>
       </c>
       <c r="B54" t="s">
+        <v>73</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="8">
+        <v>2</v>
+      </c>
+      <c r="E54" t="s">
+        <v>86</v>
+      </c>
+      <c r="F54" t="s">
         <v>87</v>
-      </c>
-      <c r="C54" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D54" s="8">
-        <v>2</v>
-      </c>
-      <c r="E54" t="s">
-        <v>103</v>
-      </c>
-      <c r="F54" t="s">
-        <v>102</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>7</v>
@@ -3211,519 +3137,445 @@
       </c>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="30" t="s">
-        <v>71</v>
+    <row r="55" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>108</v>
       </c>
       <c r="B55" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="8">
+        <v>2</v>
+      </c>
+      <c r="E55" t="s">
+        <v>86</v>
+      </c>
+      <c r="F55" t="s">
         <v>87</v>
-      </c>
-      <c r="C55" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D55" s="8">
-        <v>2</v>
-      </c>
-      <c r="E55" t="s">
-        <v>103</v>
-      </c>
-      <c r="F55" t="s">
-        <v>102</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H55" s="4">
+        <v>50</v>
+      </c>
+      <c r="L55" s="5"/>
+    </row>
+    <row r="56" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56"/>
+      <c r="B56"/>
+      <c r="C56" s="29"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="L56" s="5"/>
+    </row>
+    <row r="57" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>109</v>
+      </c>
+      <c r="B57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D57" s="8">
+        <v>2</v>
+      </c>
+      <c r="E57" t="s">
+        <v>89</v>
+      </c>
+      <c r="F57" t="s">
+        <v>88</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H57" s="4">
+        <v>1450</v>
+      </c>
+      <c r="I57" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J57" s="5">
+        <v>180</v>
+      </c>
+      <c r="L57" s="5"/>
+    </row>
+    <row r="58" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>109</v>
+      </c>
+      <c r="B58" t="s">
+        <v>73</v>
+      </c>
+      <c r="C58" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D58" s="8">
+        <v>2</v>
+      </c>
+      <c r="E58" t="s">
+        <v>89</v>
+      </c>
+      <c r="F58" t="s">
+        <v>88</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="4">
+        <v>50.331333333333333</v>
+      </c>
+      <c r="L58" s="5"/>
+    </row>
+    <row r="59" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" t="s">
+        <v>73</v>
+      </c>
+      <c r="C59" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D59" s="8">
+        <v>2</v>
+      </c>
+      <c r="E59" t="s">
+        <v>89</v>
+      </c>
+      <c r="F59" t="s">
+        <v>88</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H59" s="4">
+        <v>-144.39750000000001</v>
+      </c>
+      <c r="L59" s="5"/>
+    </row>
+    <row r="60" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>109</v>
+      </c>
+      <c r="B60" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D60" s="8">
+        <v>2</v>
+      </c>
+      <c r="E60" t="s">
+        <v>89</v>
+      </c>
+      <c r="F60" t="s">
+        <v>88</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H60" s="4">
         <v>38</v>
       </c>
-      <c r="L55" s="37"/>
-      <c r="M55" s="37"/>
-      <c r="N55" s="37"/>
-    </row>
-    <row r="56" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="B56" t="s">
-        <v>87</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D56" s="8">
-        <v>2</v>
-      </c>
-      <c r="E56" t="s">
-        <v>104</v>
-      </c>
-      <c r="F56" t="s">
-        <v>105</v>
-      </c>
-      <c r="G56" s="4" t="s">
+      <c r="L60" s="35"/>
+      <c r="M60" s="35"/>
+      <c r="N60" s="35"/>
+    </row>
+    <row r="61" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61"/>
+      <c r="B61"/>
+      <c r="C61" s="29"/>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="L61" s="35"/>
+      <c r="M61" s="35"/>
+      <c r="N61" s="35"/>
+    </row>
+    <row r="62" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" t="s">
+        <v>73</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62" s="8">
+        <v>2</v>
+      </c>
+      <c r="E62" t="s">
+        <v>90</v>
+      </c>
+      <c r="F62" t="s">
+        <v>91</v>
+      </c>
+      <c r="G62" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H56" s="4">
+      <c r="H62" s="4">
         <v>1450</v>
       </c>
-      <c r="I56" s="8" t="s">
+      <c r="I62" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J56" s="5">
+      <c r="J62" s="5">
         <v>250</v>
       </c>
-      <c r="L56" s="37"/>
-      <c r="M56" s="37"/>
-      <c r="N56" s="37"/>
-    </row>
-    <row r="57" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B57" t="s">
-        <v>87</v>
-      </c>
-      <c r="C57" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D57" s="8">
-        <v>2</v>
-      </c>
-      <c r="E57" t="s">
-        <v>104</v>
-      </c>
-      <c r="F57" t="s">
-        <v>105</v>
-      </c>
-      <c r="G57" s="4" t="s">
+      <c r="L62" s="35"/>
+      <c r="M62" s="35"/>
+      <c r="N62" s="35"/>
+    </row>
+    <row r="63" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D63" s="8">
+        <v>2</v>
+      </c>
+      <c r="E63" t="s">
+        <v>90</v>
+      </c>
+      <c r="F63" t="s">
+        <v>91</v>
+      </c>
+      <c r="G63" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H57" s="4">
+      <c r="H63" s="4">
         <v>50.331333333333333</v>
       </c>
-      <c r="L57" s="37"/>
-      <c r="M57" s="37"/>
-      <c r="N57" s="37"/>
-    </row>
-    <row r="58" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B58" t="s">
-        <v>87</v>
-      </c>
-      <c r="C58" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D58" s="8">
-        <v>2</v>
-      </c>
-      <c r="E58" t="s">
-        <v>104</v>
-      </c>
-      <c r="F58" t="s">
-        <v>105</v>
-      </c>
-      <c r="G58" s="4" t="s">
+      <c r="L63" s="35"/>
+      <c r="M63" s="35"/>
+      <c r="N63" s="35"/>
+    </row>
+    <row r="64" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>110</v>
+      </c>
+      <c r="B64" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D64" s="8">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s">
+        <v>90</v>
+      </c>
+      <c r="F64" t="s">
+        <v>91</v>
+      </c>
+      <c r="G64" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H58" s="4">
+      <c r="H64" s="4">
         <v>-144.39750000000001</v>
       </c>
-      <c r="L58" s="37"/>
-      <c r="M58" s="37"/>
-      <c r="N58" s="37"/>
-    </row>
-    <row r="59" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B59" t="s">
-        <v>87</v>
-      </c>
-      <c r="C59" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D59" s="8">
-        <v>2</v>
-      </c>
-      <c r="E59" t="s">
-        <v>104</v>
-      </c>
-      <c r="F59" t="s">
-        <v>105</v>
-      </c>
-      <c r="G59" s="4" t="s">
+      <c r="L64" s="35"/>
+      <c r="M64" s="35"/>
+      <c r="N64" s="35"/>
+    </row>
+    <row r="65" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" t="s">
+        <v>73</v>
+      </c>
+      <c r="C65" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D65" s="8">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s">
+        <v>90</v>
+      </c>
+      <c r="F65" t="s">
+        <v>91</v>
+      </c>
+      <c r="G65" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H59" s="4">
+      <c r="H65" s="4">
         <v>40</v>
       </c>
-      <c r="L59" s="37"/>
-      <c r="M59" s="37"/>
-      <c r="N59" s="37"/>
-    </row>
-    <row r="60" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="B60" t="s">
-        <v>87</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D60" s="8">
-        <v>2</v>
-      </c>
-      <c r="E60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F60" t="s">
-        <v>106</v>
-      </c>
-      <c r="G60" s="4" t="s">
+      <c r="L65" s="35"/>
+      <c r="M65" s="35"/>
+      <c r="N65" s="35"/>
+    </row>
+    <row r="66" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66"/>
+      <c r="B66"/>
+      <c r="C66" s="29"/>
+      <c r="E66"/>
+      <c r="F66"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="L66" s="35"/>
+      <c r="M66" s="35"/>
+      <c r="N66" s="35"/>
+    </row>
+    <row r="67" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>112</v>
+      </c>
+      <c r="B67" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D67" s="8">
+        <v>2</v>
+      </c>
+      <c r="E67" t="s">
+        <v>93</v>
+      </c>
+      <c r="F67" t="s">
+        <v>92</v>
+      </c>
+      <c r="G67" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H60" s="4">
+      <c r="H67" s="4">
         <v>1450</v>
       </c>
-      <c r="I60" s="8" t="s">
+      <c r="I67" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J60" s="5">
+      <c r="J67" s="5">
         <v>350</v>
       </c>
-      <c r="L60" s="37"/>
-      <c r="M60" s="37"/>
-      <c r="N60" s="37"/>
-    </row>
-    <row r="61" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="B61" t="s">
-        <v>87</v>
-      </c>
-      <c r="C61" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D61" s="8">
-        <v>2</v>
-      </c>
-      <c r="E61" t="s">
-        <v>107</v>
-      </c>
-      <c r="F61" t="s">
-        <v>106</v>
-      </c>
-      <c r="G61" s="4" t="s">
+      <c r="L67" s="35"/>
+      <c r="M67" s="35"/>
+      <c r="N67" s="35"/>
+    </row>
+    <row r="68" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>112</v>
+      </c>
+      <c r="B68" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D68" s="8">
+        <v>2</v>
+      </c>
+      <c r="E68" t="s">
+        <v>93</v>
+      </c>
+      <c r="F68" t="s">
+        <v>92</v>
+      </c>
+      <c r="G68" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H61" s="4">
+      <c r="H68" s="4">
         <v>50.331333333333333</v>
       </c>
-      <c r="L61" s="37"/>
-      <c r="M61" s="37"/>
-      <c r="N61" s="37"/>
-    </row>
-    <row r="62" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="B62" t="s">
-        <v>87</v>
-      </c>
-      <c r="C62" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D62" s="8">
-        <v>2</v>
-      </c>
-      <c r="E62" t="s">
-        <v>107</v>
-      </c>
-      <c r="F62" t="s">
-        <v>106</v>
-      </c>
-      <c r="G62" s="4" t="s">
+      <c r="L68" s="35"/>
+      <c r="M68" s="35"/>
+      <c r="N68" s="35"/>
+    </row>
+    <row r="69" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>112</v>
+      </c>
+      <c r="B69" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D69" s="8">
+        <v>2</v>
+      </c>
+      <c r="E69" t="s">
+        <v>93</v>
+      </c>
+      <c r="F69" t="s">
+        <v>92</v>
+      </c>
+      <c r="G69" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H62" s="4">
+      <c r="H69" s="4">
         <v>-144.39750000000001</v>
       </c>
-      <c r="L62" s="37"/>
-      <c r="M62" s="37"/>
-      <c r="N62" s="37"/>
-    </row>
-    <row r="63" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="B63" t="s">
-        <v>87</v>
-      </c>
-      <c r="C63" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D63" s="8">
-        <v>2</v>
-      </c>
-      <c r="E63" t="s">
-        <v>107</v>
-      </c>
-      <c r="F63" t="s">
-        <v>106</v>
-      </c>
-      <c r="G63" s="4" t="s">
+      <c r="L69" s="35"/>
+      <c r="M69" s="35"/>
+      <c r="N69" s="35"/>
+    </row>
+    <row r="70" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" s="8">
+        <v>2</v>
+      </c>
+      <c r="E70" t="s">
+        <v>93</v>
+      </c>
+      <c r="F70" t="s">
+        <v>92</v>
+      </c>
+      <c r="G70" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H63" s="4">
+      <c r="H70" s="4">
         <v>39</v>
       </c>
-      <c r="L63" s="37"/>
-      <c r="M63" s="37"/>
-      <c r="N63" s="37"/>
-    </row>
-    <row r="64" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="B64" t="s">
-        <v>87</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D64" s="8">
-        <v>2</v>
-      </c>
-      <c r="E64" t="s">
-        <v>109</v>
-      </c>
-      <c r="F64" t="s">
-        <v>108</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H64" s="4">
-        <v>1450</v>
-      </c>
-      <c r="I64" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J64" s="5">
-        <v>501</v>
-      </c>
-      <c r="L64" s="37"/>
-      <c r="M64" s="37"/>
-      <c r="N64" s="37"/>
-    </row>
-    <row r="65" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B65" t="s">
-        <v>87</v>
-      </c>
-      <c r="C65" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D65" s="8">
-        <v>2</v>
-      </c>
-      <c r="E65" t="s">
-        <v>109</v>
-      </c>
-      <c r="F65" t="s">
-        <v>108</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H65" s="4">
-        <v>50.331333333333333</v>
-      </c>
-      <c r="L65" s="37"/>
-      <c r="M65" s="37"/>
-      <c r="N65" s="37"/>
-    </row>
-    <row r="66" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B66" t="s">
-        <v>87</v>
-      </c>
-      <c r="C66" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D66" s="8">
-        <v>2</v>
-      </c>
-      <c r="E66" t="s">
-        <v>109</v>
-      </c>
-      <c r="F66" t="s">
-        <v>108</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H66" s="4">
-        <v>-144.39750000000001</v>
-      </c>
-      <c r="L66" s="37"/>
-      <c r="M66" s="37"/>
-      <c r="N66" s="37"/>
-    </row>
-    <row r="67" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B67" t="s">
-        <v>87</v>
-      </c>
-      <c r="C67" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D67" s="8">
-        <v>2</v>
-      </c>
-      <c r="E67" t="s">
-        <v>109</v>
-      </c>
-      <c r="F67" t="s">
-        <v>108</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H67" s="4">
-        <v>23</v>
-      </c>
-      <c r="L67" s="5"/>
-    </row>
-    <row r="68" spans="1:14" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="B68" t="s">
-        <v>87</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D68" s="8">
-        <v>2</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="L70" s="35"/>
+      <c r="M70" s="35"/>
+      <c r="N70" s="35"/>
+    </row>
+    <row r="71" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71"/>
+      <c r="B71"/>
+      <c r="C71" s="29"/>
+      <c r="E71"/>
+      <c r="F71"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="L71" s="35"/>
+      <c r="M71" s="35"/>
+      <c r="N71" s="35"/>
+    </row>
+    <row r="72" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>111</v>
       </c>
-      <c r="F68" t="s">
-        <v>110</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H68" s="4">
-        <v>5076</v>
-      </c>
-      <c r="I68" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="J68" s="34">
-        <v>748</v>
-      </c>
-      <c r="L68" s="34"/>
-    </row>
-    <row r="69" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="B69" t="s">
-        <v>87</v>
-      </c>
-      <c r="C69" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="D69" s="8">
-        <v>2</v>
-      </c>
-      <c r="E69" t="s">
-        <v>111</v>
-      </c>
-      <c r="F69" t="s">
-        <v>110</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H69" s="4">
-        <v>50.331333333333333</v>
-      </c>
-      <c r="L69" s="5"/>
-    </row>
-    <row r="70" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="B70" t="s">
-        <v>87</v>
-      </c>
-      <c r="C70" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="D70" s="8">
-        <v>2</v>
-      </c>
-      <c r="E70" t="s">
-        <v>111</v>
-      </c>
-      <c r="F70" t="s">
-        <v>110</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H70" s="4">
-        <v>-144.39750000000001</v>
-      </c>
-      <c r="L70" s="5"/>
-    </row>
-    <row r="71" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="B71" t="s">
-        <v>87</v>
-      </c>
-      <c r="C71" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="D71" s="8">
-        <v>2</v>
-      </c>
-      <c r="E71" t="s">
-        <v>111</v>
-      </c>
-      <c r="F71" t="s">
-        <v>110</v>
-      </c>
-      <c r="G71" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H71" s="4">
-        <v>28</v>
-      </c>
-      <c r="L71" s="5"/>
-    </row>
-    <row r="72" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="31" t="s">
-        <v>76</v>
-      </c>
       <c r="B72" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>48</v>
@@ -3732,31 +3584,33 @@
         <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="F72" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H72" s="4">
-        <v>5076</v>
+        <v>1450</v>
       </c>
       <c r="I72" s="8" t="s">
         <v>14</v>
       </c>
       <c r="J72" s="5">
-        <v>999</v>
-      </c>
-      <c r="L72" s="5"/>
-    </row>
-    <row r="73" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="30" t="s">
-        <v>76</v>
+        <v>501</v>
+      </c>
+      <c r="L72" s="35"/>
+      <c r="M72" s="35"/>
+      <c r="N72" s="35"/>
+    </row>
+    <row r="73" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>111</v>
       </c>
       <c r="B73" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C73" s="29" t="s">
         <v>48</v>
@@ -3765,10 +3619,10 @@
         <v>2</v>
       </c>
       <c r="E73" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="F73" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>6</v>
@@ -3776,14 +3630,16 @@
       <c r="H73" s="4">
         <v>50.331333333333333</v>
       </c>
-      <c r="L73" s="5"/>
-    </row>
-    <row r="74" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="30" t="s">
-        <v>76</v>
+      <c r="L73" s="35"/>
+      <c r="M73" s="35"/>
+      <c r="N73" s="35"/>
+    </row>
+    <row r="74" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>111</v>
       </c>
       <c r="B74" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C74" s="29" t="s">
         <v>48</v>
@@ -3792,10 +3648,10 @@
         <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="F74" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>7</v>
@@ -3803,14 +3659,16 @@
       <c r="H74" s="4">
         <v>-144.39750000000001</v>
       </c>
-      <c r="L74" s="5"/>
-    </row>
-    <row r="75" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="30" t="s">
-        <v>76</v>
+      <c r="L74" s="35"/>
+      <c r="M74" s="35"/>
+      <c r="N74" s="35"/>
+    </row>
+    <row r="75" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>111</v>
       </c>
       <c r="B75" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C75" s="29" t="s">
         <v>48</v>
@@ -3819,229 +3677,510 @@
         <v>2</v>
       </c>
       <c r="E75" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="F75" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H75" s="4">
+        <v>23</v>
+      </c>
+      <c r="L75" s="5"/>
+    </row>
+    <row r="76" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76"/>
+      <c r="B76"/>
+      <c r="C76" s="29"/>
+      <c r="E76"/>
+      <c r="F76"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="L76" s="5"/>
+    </row>
+    <row r="77" spans="1:14" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>113</v>
+      </c>
+      <c r="B77" t="s">
+        <v>73</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D77" s="8">
+        <v>2</v>
+      </c>
+      <c r="E77" t="s">
+        <v>97</v>
+      </c>
+      <c r="F77" t="s">
+        <v>96</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H77" s="4">
+        <v>5076</v>
+      </c>
+      <c r="I77" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="J77" s="33">
+        <v>748</v>
+      </c>
+      <c r="L77" s="33"/>
+    </row>
+    <row r="78" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>113</v>
+      </c>
+      <c r="B78" t="s">
+        <v>73</v>
+      </c>
+      <c r="C78" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D78" s="8">
+        <v>2</v>
+      </c>
+      <c r="E78" t="s">
+        <v>97</v>
+      </c>
+      <c r="F78" t="s">
+        <v>96</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H78" s="4">
+        <v>50.331333333333333</v>
+      </c>
+      <c r="L78" s="5"/>
+    </row>
+    <row r="79" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>113</v>
+      </c>
+      <c r="B79" t="s">
+        <v>73</v>
+      </c>
+      <c r="C79" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D79" s="8">
+        <v>2</v>
+      </c>
+      <c r="E79" t="s">
+        <v>97</v>
+      </c>
+      <c r="F79" t="s">
+        <v>96</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H79" s="4">
+        <v>-144.39750000000001</v>
+      </c>
+      <c r="L79" s="5"/>
+    </row>
+    <row r="80" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>113</v>
+      </c>
+      <c r="B80" t="s">
+        <v>73</v>
+      </c>
+      <c r="C80" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D80" s="8">
+        <v>2</v>
+      </c>
+      <c r="E80" t="s">
+        <v>97</v>
+      </c>
+      <c r="F80" t="s">
+        <v>96</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H80" s="4">
+        <v>28</v>
+      </c>
+      <c r="L80" s="5"/>
+    </row>
+    <row r="81" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81"/>
+      <c r="B81"/>
+      <c r="C81" s="32"/>
+      <c r="E81"/>
+      <c r="F81"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+      <c r="L81" s="5"/>
+    </row>
+    <row r="82" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>114</v>
+      </c>
+      <c r="B82" t="s">
+        <v>73</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D82" s="8">
+        <v>2</v>
+      </c>
+      <c r="E82" t="s">
+        <v>99</v>
+      </c>
+      <c r="F82" t="s">
+        <v>98</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H82" s="4">
+        <v>5076</v>
+      </c>
+      <c r="I82" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J82" s="5">
+        <v>999</v>
+      </c>
+      <c r="L82" s="5"/>
+    </row>
+    <row r="83" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>114</v>
+      </c>
+      <c r="B83" t="s">
+        <v>73</v>
+      </c>
+      <c r="C83" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D83" s="8">
+        <v>2</v>
+      </c>
+      <c r="E83" t="s">
+        <v>99</v>
+      </c>
+      <c r="F83" t="s">
+        <v>98</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H83" s="4">
+        <v>50.331333333333333</v>
+      </c>
+      <c r="L83" s="5"/>
+    </row>
+    <row r="84" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>114</v>
+      </c>
+      <c r="B84" t="s">
+        <v>73</v>
+      </c>
+      <c r="C84" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D84" s="8">
+        <v>2</v>
+      </c>
+      <c r="E84" t="s">
+        <v>99</v>
+      </c>
+      <c r="F84" t="s">
+        <v>98</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H84" s="4">
+        <v>-144.39750000000001</v>
+      </c>
+      <c r="L84" s="5"/>
+    </row>
+    <row r="85" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>114</v>
+      </c>
+      <c r="B85" t="s">
+        <v>73</v>
+      </c>
+      <c r="C85" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D85" s="8">
+        <v>2</v>
+      </c>
+      <c r="E85" t="s">
+        <v>99</v>
+      </c>
+      <c r="F85" t="s">
+        <v>98</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H85" s="4">
         <v>80</v>
       </c>
-      <c r="L75" s="5"/>
-    </row>
-    <row r="76" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B76" t="s">
-        <v>87</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D76" s="8">
-        <v>2</v>
-      </c>
-      <c r="E76" t="s">
+      <c r="L85" s="5"/>
+    </row>
+    <row r="86" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86"/>
+      <c r="B86"/>
+      <c r="C86" s="29"/>
+      <c r="E86"/>
+      <c r="F86"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
+      <c r="L86" s="5"/>
+    </row>
+    <row r="87" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>115</v>
       </c>
-      <c r="F76" t="s">
-        <v>114</v>
-      </c>
-      <c r="G76" s="4" t="s">
+      <c r="B87" t="s">
+        <v>73</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D87" s="8">
+        <v>2</v>
+      </c>
+      <c r="E87" t="s">
+        <v>101</v>
+      </c>
+      <c r="F87" t="s">
+        <v>100</v>
+      </c>
+      <c r="G87" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H76" s="4">
+      <c r="H87" s="4">
         <v>5076</v>
       </c>
-      <c r="I76" s="8" t="s">
+      <c r="I87" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J76" s="5">
+      <c r="J87" s="5">
         <v>1501</v>
       </c>
-      <c r="L76" s="5"/>
-    </row>
-    <row r="77" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B77" t="s">
-        <v>87</v>
-      </c>
-      <c r="C77" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D77" s="8">
-        <v>2</v>
-      </c>
-      <c r="E77" t="s">
+      <c r="L87" s="5"/>
+    </row>
+    <row r="88" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>115</v>
       </c>
-      <c r="F77" t="s">
-        <v>114</v>
-      </c>
-      <c r="G77" s="4" t="s">
+      <c r="B88" t="s">
+        <v>73</v>
+      </c>
+      <c r="C88" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D88" s="8">
+        <v>2</v>
+      </c>
+      <c r="E88" t="s">
+        <v>101</v>
+      </c>
+      <c r="F88" t="s">
+        <v>100</v>
+      </c>
+      <c r="G88" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H77" s="4">
+      <c r="H88" s="4">
         <v>50.331333333333333</v>
       </c>
-      <c r="L77" s="5"/>
-    </row>
-    <row r="78" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B78" t="s">
-        <v>87</v>
-      </c>
-      <c r="C78" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D78" s="8">
-        <v>2</v>
-      </c>
-      <c r="E78" t="s">
+      <c r="L88" s="5"/>
+    </row>
+    <row r="89" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>115</v>
       </c>
-      <c r="F78" t="s">
-        <v>114</v>
-      </c>
-      <c r="G78" s="4" t="s">
+      <c r="B89" t="s">
+        <v>73</v>
+      </c>
+      <c r="C89" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D89" s="8">
+        <v>2</v>
+      </c>
+      <c r="E89" t="s">
+        <v>101</v>
+      </c>
+      <c r="F89" t="s">
+        <v>100</v>
+      </c>
+      <c r="G89" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H78" s="4">
+      <c r="H89" s="4">
         <v>-144.39750000000001</v>
       </c>
-      <c r="L78" s="5"/>
-    </row>
-    <row r="79" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B79" t="s">
-        <v>87</v>
-      </c>
-      <c r="C79" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D79" s="8">
-        <v>2</v>
-      </c>
-      <c r="E79" t="s">
+      <c r="L89" s="5"/>
+    </row>
+    <row r="90" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>115</v>
       </c>
-      <c r="F79" t="s">
-        <v>114</v>
-      </c>
-      <c r="G79" s="4" t="s">
+      <c r="B90" t="s">
+        <v>73</v>
+      </c>
+      <c r="C90" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D90" s="8">
+        <v>2</v>
+      </c>
+      <c r="E90" t="s">
+        <v>101</v>
+      </c>
+      <c r="F90" t="s">
+        <v>100</v>
+      </c>
+      <c r="G90" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H79" s="4">
+      <c r="H90" s="4">
         <v>3</v>
       </c>
-      <c r="L79" s="5"/>
-    </row>
-    <row r="80" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A80" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="B80" t="s">
-        <v>87</v>
-      </c>
-      <c r="C80" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="D80" s="42">
-        <v>2</v>
-      </c>
-      <c r="E80" s="42"/>
-      <c r="F80" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="L80" s="5"/>
-    </row>
-    <row r="81" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A81" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="B81" t="s">
-        <v>87</v>
-      </c>
-      <c r="C81" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="D81" s="42">
-        <v>2</v>
-      </c>
-      <c r="E81" s="42"/>
-      <c r="F81" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="G81" s="20"/>
-      <c r="H81" s="20"/>
-      <c r="I81" s="21"/>
-      <c r="J81" s="20"/>
-      <c r="K81" s="20"/>
-      <c r="L81" s="20"/>
-      <c r="M81" s="20"/>
-      <c r="N81" s="20"/>
-      <c r="O81" s="20"/>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A82" s="20"/>
-      <c r="B82" s="20"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="21"/>
-      <c r="E82" s="21"/>
-      <c r="F82" s="20"/>
-      <c r="G82" s="20"/>
-      <c r="H82" s="20"/>
-      <c r="I82" s="21"/>
-      <c r="J82" s="20"/>
-      <c r="K82" s="20"/>
-      <c r="L82" s="20"/>
-      <c r="M82" s="20"/>
-      <c r="N82" s="20"/>
-      <c r="O82" s="20"/>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A83" s="20"/>
-      <c r="B83" s="20"/>
-      <c r="C83" s="20"/>
-      <c r="D83" s="21"/>
-      <c r="E83" s="21"/>
-      <c r="F83" s="20"/>
-      <c r="G83" s="20"/>
-      <c r="H83" s="20"/>
-      <c r="I83" s="21"/>
-      <c r="J83" s="20"/>
-      <c r="K83" s="20"/>
-      <c r="L83" s="20"/>
-      <c r="M83" s="20"/>
-      <c r="N83" s="20"/>
-      <c r="O83" s="20"/>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A84" s="20"/>
-      <c r="B84" s="20"/>
-      <c r="C84" s="20"/>
-      <c r="D84" s="21"/>
-      <c r="E84" s="21"/>
-      <c r="F84" s="20"/>
-      <c r="G84" s="20"/>
-      <c r="H84" s="20"/>
-      <c r="I84" s="21"/>
-      <c r="J84" s="20"/>
-      <c r="K84" s="20"/>
-      <c r="L84" s="20"/>
-      <c r="M84" s="20"/>
-      <c r="N84" s="20"/>
-      <c r="O84" s="20"/>
+      <c r="L90" s="5"/>
+    </row>
+    <row r="91" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91"/>
+      <c r="B91"/>
+      <c r="C91" s="29"/>
+      <c r="E91"/>
+      <c r="F91"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="L91" s="5"/>
+    </row>
+    <row r="92" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="B92" t="s">
+        <v>73</v>
+      </c>
+      <c r="C92" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D92" s="40">
+        <v>2</v>
+      </c>
+      <c r="E92" t="s">
+        <v>116</v>
+      </c>
+      <c r="F92" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="L92" s="5"/>
+    </row>
+    <row r="93" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="38"/>
+      <c r="B93"/>
+      <c r="C93" s="39"/>
+      <c r="D93" s="40"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="41"/>
+      <c r="L93" s="48"/>
+    </row>
+    <row r="94" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="B94" t="s">
+        <v>73</v>
+      </c>
+      <c r="C94" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D94" s="40">
+        <v>2</v>
+      </c>
+      <c r="E94" t="s">
+        <v>117</v>
+      </c>
+      <c r="F94" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="G94" s="20"/>
+      <c r="H94" s="20"/>
+      <c r="I94" s="21"/>
+      <c r="J94" s="20"/>
+      <c r="K94" s="20"/>
+      <c r="L94" s="20"/>
+      <c r="M94" s="20"/>
+      <c r="N94" s="20"/>
+      <c r="O94" s="20"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A95" s="20"/>
+      <c r="B95" s="20"/>
+      <c r="C95" s="20"/>
+      <c r="D95" s="21"/>
+      <c r="E95" s="21"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="20"/>
+      <c r="H95" s="20"/>
+      <c r="I95" s="21"/>
+      <c r="J95" s="20"/>
+      <c r="K95" s="20"/>
+      <c r="L95" s="20"/>
+      <c r="M95" s="20"/>
+      <c r="N95" s="20"/>
+      <c r="O95" s="20"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96" s="20"/>
+      <c r="B96" s="20"/>
+      <c r="C96" s="20"/>
+      <c r="D96" s="21"/>
+      <c r="E96" s="21"/>
+      <c r="F96" s="20"/>
+      <c r="G96" s="20"/>
+      <c r="H96" s="20"/>
+      <c r="I96" s="21"/>
+      <c r="J96" s="20"/>
+      <c r="K96" s="20"/>
+      <c r="L96" s="20"/>
+      <c r="M96" s="20"/>
+      <c r="N96" s="20"/>
+      <c r="O96" s="20"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A97" s="20"/>
+      <c r="B97" s="20"/>
+      <c r="C97" s="20"/>
+      <c r="D97" s="21"/>
+      <c r="E97" s="21"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="20"/>
+      <c r="H97" s="20"/>
+      <c r="I97" s="21"/>
+      <c r="J97" s="20"/>
+      <c r="K97" s="20"/>
+      <c r="L97" s="20"/>
+      <c r="M97" s="20"/>
+      <c r="N97" s="20"/>
+      <c r="O97" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Corrected engineering reference designators
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GP03FLMB_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_GP03FLMB_00002.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="1950" windowWidth="24960" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="2310" yWindow="1950" windowWidth="24960" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -917,7 +917,7 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1057,9 +1057,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="134">
@@ -1517,7 +1514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1663,11 +1660,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F94" sqref="F94"/>
+      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2600,6 +2597,7 @@
       <c r="J32" s="2">
         <v>29</v>
       </c>
+      <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -2626,6 +2624,7 @@
       <c r="H33" s="4">
         <v>50.331333333333333</v>
       </c>
+      <c r="L33" s="5"/>
     </row>
     <row r="34" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -2652,6 +2651,7 @@
       <c r="H34" s="4">
         <v>-144.39750000000001</v>
       </c>
+      <c r="L34" s="5"/>
     </row>
     <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -2678,6 +2678,7 @@
       <c r="H35" s="4">
         <v>46</v>
       </c>
+      <c r="L35" s="5"/>
     </row>
     <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A36"/>
@@ -2687,6 +2688,7 @@
       <c r="F36"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
+      <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -2719,6 +2721,7 @@
       <c r="J37" s="5">
         <v>39</v>
       </c>
+      <c r="L37" s="5"/>
     </row>
     <row r="38" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -2745,6 +2748,7 @@
       <c r="H38" s="4">
         <v>50.331333333333333</v>
       </c>
+      <c r="L38" s="5"/>
     </row>
     <row r="39" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -2771,6 +2775,7 @@
       <c r="H39" s="4">
         <v>-144.39750000000001</v>
       </c>
+      <c r="L39" s="5"/>
     </row>
     <row r="40" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -2797,6 +2802,7 @@
       <c r="H40" s="4">
         <v>54</v>
       </c>
+      <c r="L40" s="5"/>
     </row>
     <row r="41" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A41"/>
@@ -2806,6 +2812,7 @@
       <c r="F41"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
+      <c r="L41" s="5"/>
     </row>
     <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -2838,6 +2845,7 @@
       <c r="J42" s="5">
         <v>59</v>
       </c>
+      <c r="L42" s="5"/>
     </row>
     <row r="43" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -2864,6 +2872,7 @@
       <c r="H43" s="4">
         <v>50.331333333333333</v>
       </c>
+      <c r="L43" s="5"/>
     </row>
     <row r="44" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -2890,6 +2899,7 @@
       <c r="H44" s="4">
         <v>-144.39750000000001</v>
       </c>
+      <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -2916,6 +2926,7 @@
       <c r="H45" s="4">
         <v>53</v>
       </c>
+      <c r="L45" s="5"/>
     </row>
     <row r="46" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A46"/>
@@ -2925,6 +2936,7 @@
       <c r="F46"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
+      <c r="L46" s="5"/>
     </row>
     <row r="47" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -3286,7 +3298,7 @@
       <c r="H60" s="4">
         <v>38</v>
       </c>
-      <c r="L60" s="35"/>
+      <c r="L60" s="5"/>
       <c r="M60" s="35"/>
       <c r="N60" s="35"/>
     </row>
@@ -3298,7 +3310,7 @@
       <c r="F61"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
-      <c r="L61" s="35"/>
+      <c r="L61" s="5"/>
       <c r="M61" s="35"/>
       <c r="N61" s="35"/>
     </row>
@@ -3333,7 +3345,7 @@
       <c r="J62" s="5">
         <v>250</v>
       </c>
-      <c r="L62" s="35"/>
+      <c r="L62" s="5"/>
       <c r="M62" s="35"/>
       <c r="N62" s="35"/>
     </row>
@@ -3362,7 +3374,7 @@
       <c r="H63" s="4">
         <v>50.331333333333333</v>
       </c>
-      <c r="L63" s="35"/>
+      <c r="L63" s="5"/>
       <c r="M63" s="35"/>
       <c r="N63" s="35"/>
     </row>
@@ -3391,7 +3403,7 @@
       <c r="H64" s="4">
         <v>-144.39750000000001</v>
       </c>
-      <c r="L64" s="35"/>
+      <c r="L64" s="5"/>
       <c r="M64" s="35"/>
       <c r="N64" s="35"/>
     </row>
@@ -3420,7 +3432,7 @@
       <c r="H65" s="4">
         <v>40</v>
       </c>
-      <c r="L65" s="35"/>
+      <c r="L65" s="5"/>
       <c r="M65" s="35"/>
       <c r="N65" s="35"/>
     </row>
@@ -3432,7 +3444,7 @@
       <c r="F66"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
-      <c r="L66" s="35"/>
+      <c r="L66" s="5"/>
       <c r="M66" s="35"/>
       <c r="N66" s="35"/>
     </row>
@@ -3467,7 +3479,7 @@
       <c r="J67" s="5">
         <v>350</v>
       </c>
-      <c r="L67" s="35"/>
+      <c r="L67" s="5"/>
       <c r="M67" s="35"/>
       <c r="N67" s="35"/>
     </row>
@@ -3496,7 +3508,7 @@
       <c r="H68" s="4">
         <v>50.331333333333333</v>
       </c>
-      <c r="L68" s="35"/>
+      <c r="L68" s="5"/>
       <c r="M68" s="35"/>
       <c r="N68" s="35"/>
     </row>
@@ -3525,7 +3537,7 @@
       <c r="H69" s="4">
         <v>-144.39750000000001</v>
       </c>
-      <c r="L69" s="35"/>
+      <c r="L69" s="5"/>
       <c r="M69" s="35"/>
       <c r="N69" s="35"/>
     </row>
@@ -3554,7 +3566,7 @@
       <c r="H70" s="4">
         <v>39</v>
       </c>
-      <c r="L70" s="35"/>
+      <c r="L70" s="5"/>
       <c r="M70" s="35"/>
       <c r="N70" s="35"/>
     </row>
@@ -3566,7 +3578,7 @@
       <c r="F71"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
-      <c r="L71" s="35"/>
+      <c r="L71" s="5"/>
       <c r="M71" s="35"/>
       <c r="N71" s="35"/>
     </row>
@@ -3601,7 +3613,7 @@
       <c r="J72" s="5">
         <v>501</v>
       </c>
-      <c r="L72" s="35"/>
+      <c r="L72" s="5"/>
       <c r="M72" s="35"/>
       <c r="N72" s="35"/>
     </row>
@@ -3630,7 +3642,7 @@
       <c r="H73" s="4">
         <v>50.331333333333333</v>
       </c>
-      <c r="L73" s="35"/>
+      <c r="L73" s="5"/>
       <c r="M73" s="35"/>
       <c r="N73" s="35"/>
     </row>
@@ -3659,7 +3671,7 @@
       <c r="H74" s="4">
         <v>-144.39750000000001</v>
       </c>
-      <c r="L74" s="35"/>
+      <c r="L74" s="5"/>
       <c r="M74" s="35"/>
       <c r="N74" s="35"/>
     </row>
@@ -3731,7 +3743,7 @@
       <c r="J77" s="33">
         <v>748</v>
       </c>
-      <c r="L77" s="33"/>
+      <c r="L77" s="5"/>
     </row>
     <row r="78" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
@@ -4100,7 +4112,7 @@
       <c r="D93" s="40"/>
       <c r="E93" s="2"/>
       <c r="F93" s="41"/>
-      <c r="L93" s="48"/>
+      <c r="L93" s="5"/>
     </row>
     <row r="94" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="38" t="s">
@@ -4126,7 +4138,7 @@
       <c r="I94" s="21"/>
       <c r="J94" s="20"/>
       <c r="K94" s="20"/>
-      <c r="L94" s="20"/>
+      <c r="L94" s="5"/>
       <c r="M94" s="20"/>
       <c r="N94" s="20"/>
       <c r="O94" s="20"/>

</xml_diff>